<commit_message>
Correção das URLs - retirada do parâmetro no final
</commit_message>
<xml_diff>
--- a/Entrega_Parcial_1/DE_PARA_API_URL_00.xlsx
+++ b/Entrega_Parcial_1/DE_PARA_API_URL_00.xlsx
@@ -30,15 +30,9 @@
     <t>CEP</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/cep/v2/{cep}</t>
-  </si>
-  <si>
     <t>DDD</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/ddd/v1/{ddd}</t>
-  </si>
-  <si>
     <t>Banco</t>
   </si>
   <si>
@@ -48,43 +42,49 @@
     <t>CNPJ</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/cnpj/v1/{cnpj}</t>
-  </si>
-  <si>
     <t>IBGE</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/ibge/municipios/v1/{siglaUF}?providers=dados-abertos-br,gov,wikipedia</t>
-  </si>
-  <si>
     <t>Feriados Nacionais</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/feriados/v1/{ano}</t>
-  </si>
-  <si>
     <t>Tabela FIPE</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/fipe/marcas/v1/{tipoVeiculo}</t>
-  </si>
-  <si>
     <t>ISBN</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/isbn/v1/{isbn}</t>
-  </si>
-  <si>
     <t>Registros de domínio BR</t>
   </si>
   <si>
-    <t>https://brasilapi.com.br/api/registrobr/v1/{domain}</t>
-  </si>
-  <si>
     <t>Taxas</t>
   </si>
   <si>
     <t>https://brasilapi.com.br/api/taxas/v1</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/cep/v2</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/ddd/v1</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/cnpj/v1</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/ibge/municipios/v1</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/feriados/v1</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/fipe/marcas/v1</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/registrobr/v1</t>
+  </si>
+  <si>
+    <t>https://brasilapi.com.br/api/isbn/v1</t>
   </si>
 </sst>
 </file>
@@ -894,7 +894,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,79 +912,79 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>